<commit_message>
debugging and interface changes
</commit_message>
<xml_diff>
--- a/data/admin_report.xlsx
+++ b/data/admin_report.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Bookings" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>booking_id</t>
+          <t>appointment_id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -478,40 +478,84 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>9999</t>
+          <t>APP-20250907-8C2F36</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Deivyansh</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>9999</v>
+          <t>Deivyansh Singh</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>patient_id</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2002-07-27</t>
+          <t>27-07-2002</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>Provided</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Dr. Ben Adams</t>
+          <t>Dr. Brenda Roberson</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-09-07T09:30:00</t>
+          <t>2025-09-08T08:15:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-09-06T12:43:58.564014</t>
+          <t>2025-09-07T17:42:02.928026</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>APP-20250907-C4CD42</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Deivyansh Singh</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>PAT-678A7BFF</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>27-07-2002</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Provided</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Dr. Alex Davis</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-09-08T10:30:00</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2025-09-07T18:33:48.556557</t>
         </is>
       </c>
     </row>

</xml_diff>